<commit_message>
7-11 1D eng word scaling analysis
</commit_message>
<xml_diff>
--- a/2 - Language (Words)/[7-11] Word Scaling Analysis (distance)/Parameter Tables/Aggregate-Parameters-for_English_Scaling.xlsx
+++ b/2 - Language (Words)/[7-11] Word Scaling Analysis (distance)/Parameter Tables/Aggregate-Parameters-for_English_Scaling.xlsx
@@ -165,46 +165,46 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>1.896390451723762</v>
+        <v>1.7188091074009018</v>
       </c>
       <c r="B2" s="0">
-        <v>0.42101585048140677</v>
+        <v>0.36700743467069175</v>
       </c>
       <c r="C2" s="0">
-        <v>-74.993898378305659</v>
+        <v>-54.200260732023125</v>
       </c>
       <c r="D2" s="0">
-        <v>4.534217318468694</v>
+        <v>3.5524155020463346</v>
       </c>
       <c r="E2" s="0">
-        <v>523.56216958893515</v>
+        <v>509.78706515910977</v>
       </c>
       <c r="F2" s="0">
-        <v>10.10394780819016</v>
+        <v>8.6483402685236808</v>
       </c>
       <c r="G2" s="0">
-        <v>720.49639500260696</v>
+        <v>660.57699420414178</v>
       </c>
       <c r="H2" s="0">
-        <v>9.8999992009817372</v>
+        <v>7.7851433262835137</v>
       </c>
       <c r="I2" s="0">
-        <v>7.967860890549213</v>
+        <v>7.8752251000398106</v>
       </c>
       <c r="J2" s="0">
-        <v>1.1382658415070304</v>
+        <v>1.1250321571485444</v>
       </c>
       <c r="K2" s="0">
-        <v>0.82400496274432911</v>
+        <v>0.45460950501875674</v>
       </c>
       <c r="L2" s="0">
-        <v>0.82400496274432911</v>
+        <v>0.45460950501875674</v>
       </c>
       <c r="M2" s="0">
-        <v>0.56130392244882343</v>
+        <v>0.63581382624014027</v>
       </c>
       <c r="N2" s="0">
-        <v>-0.96332797949972648</v>
+        <v>-0.97228988306570696</v>
       </c>
     </row>
   </sheetData>

</xml_diff>